<commit_message>
update isotope corrections and summary data
</commit_message>
<xml_diff>
--- a/data_raw/Summary_metadata/Oman_Geochem_2012-2019_14CH4.xlsx
+++ b/data_raw/Summary_metadata/Oman_Geochem_2012-2019_14CH4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melo.d/Desktop/Research/thesis_prep/manuscripts/Oman-14CH4/Oman-14CH4/data_raw/Summary_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2551BA0E-19C7-6B4E-BBC2-8CC3426E91D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219541B9-DC3A-0042-B357-B8C8FACABA16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="37800" windowHeight="20800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="11480" windowWidth="37800" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6653" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6655" uniqueCount="296">
   <si>
     <t>NSHQ3B</t>
   </si>
@@ -9328,11 +9328,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB11BABD-C7A2-BB46-B0A7-190733773DAE}">
   <dimension ref="A1:IE59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="11" ySplit="1" topLeftCell="GM2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="11" ySplit="1" topLeftCell="GQ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="GO57" sqref="GO57"/>
+      <selection pane="bottomRight" activeCell="GS9" sqref="GS9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10840,7 +10840,7 @@
         <v>7.2103059936602198</v>
       </c>
       <c r="GS2" s="5">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="GT2" s="5" t="s">
         <v>14</v>
@@ -10870,7 +10870,7 @@
         <v>-263.11376307990099</v>
       </c>
       <c r="HC2" s="27">
-        <v>4.0671817154160497</v>
+        <v>5</v>
       </c>
       <c r="HD2" s="5" t="s">
         <v>14</v>
@@ -11559,7 +11559,7 @@
         <v>4.4758942061459503</v>
       </c>
       <c r="GS3" s="5">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="GT3" s="5" t="s">
         <v>14</v>
@@ -11589,7 +11589,7 @@
         <v>-250.60658602378999</v>
       </c>
       <c r="HC3" s="27">
-        <v>4.0288337008783399</v>
+        <v>5</v>
       </c>
       <c r="HD3" s="5" t="s">
         <v>14</v>
@@ -12996,8 +12996,8 @@
       <c r="GR5" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="GS5" s="5">
-        <v>0.6</v>
+      <c r="GS5" s="57" t="s">
+        <v>14</v>
       </c>
       <c r="GT5" s="5" t="s">
         <v>14</v>
@@ -13716,7 +13716,7 @@
         <v>-21.783919930846402</v>
       </c>
       <c r="GS6" s="5">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="GT6" s="5" t="s">
         <v>14</v>
@@ -13746,7 +13746,7 @@
         <v>-346.62017936924701</v>
       </c>
       <c r="HC6" s="59">
-        <v>4.4800000000000004</v>
+        <v>5</v>
       </c>
       <c r="HD6" s="5" t="s">
         <v>14</v>
@@ -14435,7 +14435,7 @@
         <v>7.0372298430596798</v>
       </c>
       <c r="GS7" s="5">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="GT7" s="5" t="s">
         <v>14</v>
@@ -14465,7 +14465,7 @@
         <v>-303.86527164176402</v>
       </c>
       <c r="HC7" s="59">
-        <v>4.2838885942463296</v>
+        <v>5</v>
       </c>
       <c r="HD7" s="5" t="s">
         <v>14</v>
@@ -15151,8 +15151,8 @@
       <c r="GR8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="GS8" s="5">
-        <v>0.6</v>
+      <c r="GS8" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="GT8" s="5" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
remake isotope and well figs
</commit_message>
<xml_diff>
--- a/data_raw/Summary_metadata/Oman_Geochem_2012-2019_14CH4.xlsx
+++ b/data_raw/Summary_metadata/Oman_Geochem_2012-2019_14CH4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melo.d/Desktop/Research/thesis_prep/manuscripts/Oman-14CH4/Oman-14CH4/data_raw/Summary_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF00F7AC-B264-2B42-A7C8-A856838B9D3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69DBAC3-D25C-4041-BCBF-226F3A054CD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="37800" windowHeight="20080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9329,10 +9329,10 @@
   <dimension ref="A1:IE59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="11" ySplit="1" topLeftCell="HM2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="1" topLeftCell="HT2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="HP2" sqref="HP2"/>
+      <selection pane="bottomRight" activeCell="IA1" sqref="IA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add 2019 SiO2 colorometric data
</commit_message>
<xml_diff>
--- a/data_raw/Summary_metadata/Oman_Geochem_2012-2019_14CH4.xlsx
+++ b/data_raw/Summary_metadata/Oman_Geochem_2012-2019_14CH4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melo.d/Desktop/Research/thesis_prep/manuscripts/Oman-14CH4/Oman-14CH4/data_raw/Summary_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F466CA-D004-4A43-B024-E3B35D4B0005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6A1E1C-2797-194A-8C16-939D0F48CB16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="14080" windowWidth="38400" windowHeight="7440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="14080" windowWidth="49020" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6653" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="296">
   <si>
     <t>NSHQ3B</t>
   </si>
@@ -9329,10 +9329,10 @@
   <dimension ref="A1:IE59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="11" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="1" topLeftCell="BC2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomRight" activeCell="BF7" sqref="BF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10407,11 +10407,11 @@
       <c r="BD2" s="20">
         <v>0.11769819301987386</v>
       </c>
-      <c r="BE2" s="21" t="s">
-        <v>14</v>
+      <c r="BE2" s="21">
+        <v>2.7</v>
       </c>
       <c r="BF2" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG2" s="21" t="s">
         <v>14</v>
@@ -11126,11 +11126,11 @@
       <c r="BD3" s="20">
         <v>0.11769819301987386</v>
       </c>
-      <c r="BE3" s="21" t="s">
-        <v>14</v>
+      <c r="BE3" s="21">
+        <v>2.2000000000000002</v>
       </c>
       <c r="BF3" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG3" s="21" t="s">
         <v>14</v>
@@ -11845,11 +11845,11 @@
       <c r="BD4" s="20">
         <v>0.11769819301987386</v>
       </c>
-      <c r="BE4" s="21" t="s">
-        <v>14</v>
+      <c r="BE4" s="21">
+        <v>257.8</v>
       </c>
       <c r="BF4" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG4" s="21" t="s">
         <v>14</v>
@@ -14002,11 +14002,11 @@
       <c r="BD7" s="20">
         <v>0.11769819301987386</v>
       </c>
-      <c r="BE7" s="21" t="s">
-        <v>14</v>
+      <c r="BE7" s="21">
+        <v>12</v>
       </c>
       <c r="BF7" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG7" s="21" t="s">
         <v>14</v>

</xml_diff>